<commit_message>
fix duplicates in schools, flg_afr in school, muni
</commit_message>
<xml_diff>
--- a/data/_dictionary_13.xlsx
+++ b/data/_dictionary_13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/acfrs_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEE7088-9570-8A45-A55A-E12AE172E298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6602E40-722C-6942-864B-F2A019060BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="26620" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="7020" windowWidth="26620" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="430">
   <si>
     <t>state.abb</t>
   </si>
@@ -1292,13 +1292,31 @@
   </si>
   <si>
     <t>barnwell county consolidated school district</t>
+  </si>
+  <si>
+    <t>cook county sd 130</t>
+  </si>
+  <si>
+    <t>detroit public schools community district</t>
+  </si>
+  <si>
+    <t>detroit public schools</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Bamberg School District No. 1</t>
+  </si>
+  <si>
+    <t>ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1319,6 +1337,25 @@
       <color rgb="FF404040"/>
       <name val="Lucida Grande"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF212529"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="13.5"/>
@@ -1347,13 +1384,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1658,11 +1698,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C132" sqref="C132"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3527,7 +3567,7 @@
         <v>805550</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>67</v>
       </c>
@@ -3541,7 +3581,7 @@
         <v>802280</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>167</v>
       </c>
@@ -3555,7 +3595,7 @@
         <v>1729010</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>40</v>
       </c>
@@ -3569,7 +3609,7 @@
         <v>3412060</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>404</v>
       </c>
@@ -3581,6 +3621,106 @@
       </c>
       <c r="D132" s="2">
         <v>4501080</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C133" s="4">
+        <v>32902</v>
+      </c>
+      <c r="D133" s="4">
+        <v>1706510</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C134" s="5">
+        <v>631020</v>
+      </c>
+      <c r="D134" s="4">
+        <v>98929</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="C135" s="4">
+        <v>161679</v>
+      </c>
+      <c r="D135" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C136" s="4">
+        <v>1268305</v>
+      </c>
+      <c r="D136" s="4">
+        <v>2601103</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A137" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="C137">
+        <v>38320</v>
+      </c>
+      <c r="D137" s="4">
+        <v>4503916</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C138" s="4">
+        <v>108426</v>
+      </c>
+      <c r="D138" s="4">
+        <v>3800406</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C139" s="4">
+        <v>68028</v>
+      </c>
+      <c r="D139" s="4">
+        <v>642270</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C140" s="4">
+        <v>91083</v>
+      </c>
+      <c r="D140" s="4">
+        <v>602670</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checking extremes values per cap in school districts
</commit_message>
<xml_diff>
--- a/data/_dictionary_13.xlsx
+++ b/data/_dictionary_13.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/acfrs_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6602E40-722C-6942-864B-F2A019060BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140AF5D7-2432-2E42-B9D0-467014A71AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="7020" windowWidth="26620" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="2800" windowWidth="26620" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="438">
   <si>
     <t>state.abb</t>
   </si>
@@ -1310,13 +1323,37 @@
   </si>
   <si>
     <t>ND</t>
+  </si>
+  <si>
+    <t>Jefferson Elementary School District (San Mateo)</t>
+  </si>
+  <si>
+    <t>lakeside union</t>
+  </si>
+  <si>
+    <t>eastern aroostook regional school unit no. 39</t>
+  </si>
+  <si>
+    <t>54044</t>
+  </si>
+  <si>
+    <t>west sonoma county union high school district</t>
+  </si>
+  <si>
+    <t>91083</t>
+  </si>
+  <si>
+    <t>sequoia union high school district</t>
+  </si>
+  <si>
+    <t>146642</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1363,13 +1400,25 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF212529"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1384,7 +1433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1394,6 +1443,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1698,11 +1749,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E140"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B142" sqref="B142"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3723,6 +3774,76 @@
         <v>602670</v>
       </c>
     </row>
+    <row r="141" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A141" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="C141" s="4">
+        <v>1269433</v>
+      </c>
+      <c r="D141" s="4">
+        <v>618870</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B142" t="s">
+        <v>431</v>
+      </c>
+      <c r="C142" s="4">
+        <v>1270508</v>
+      </c>
+      <c r="D142" s="4">
+        <v>620730</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>222</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="C143" t="s">
+        <v>433</v>
+      </c>
+      <c r="D143" s="4">
+        <v>2314794</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>123</v>
+      </c>
+      <c r="B144" t="s">
+        <v>434</v>
+      </c>
+      <c r="C144" t="s">
+        <v>435</v>
+      </c>
+      <c r="D144" s="4">
+        <v>602670</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>123</v>
+      </c>
+      <c r="B145" t="s">
+        <v>436</v>
+      </c>
+      <c r="C145" t="s">
+        <v>437</v>
+      </c>
+      <c r="D145" s="4">
+        <v>636390</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update IL state;  counties, muni: adding coordinate, resolve dups
</commit_message>
<xml_diff>
--- a/data/_dictionary_13.xlsx
+++ b/data/_dictionary_13.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/acfrs_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140AF5D7-2432-2E42-B9D0-467014A71AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC933A9E-7401-754D-AC92-47B0F032AF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="2800" windowWidth="26620" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="2700" windowWidth="21020" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="436">
   <si>
     <t>state.abb</t>
   </si>
@@ -695,12 +695,6 @@
     <t>2007500</t>
   </si>
   <si>
-    <t>west elk united school district no. 282</t>
-  </si>
-  <si>
-    <t>1268609</t>
-  </si>
-  <si>
     <t>ME</t>
   </si>
   <si>
@@ -1286,9 +1280,6 @@
     <t>adams county school district no. 14</t>
   </si>
   <si>
-    <t>eastern aroostook regional school unit no. 39</t>
-  </si>
-  <si>
     <t>northwestern local school district (clark county)</t>
   </si>
   <si>
@@ -1347,13 +1338,16 @@
   </si>
   <si>
     <t>146642</t>
+  </si>
+  <si>
+    <t>AR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1406,6 +1400,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1433,7 +1433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1445,6 +1445,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1749,16 +1750,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B151" sqref="B151"/>
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="2" max="2" width="66.5" customWidth="1"/>
     <col min="3" max="3" width="36.1640625" customWidth="1"/>
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
   </cols>
@@ -2658,270 +2659,256 @@
         <v>219</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>210</v>
-      </c>
-      <c r="B60" t="s">
-        <v>220</v>
-      </c>
-      <c r="C60" t="s">
-        <v>221</v>
-      </c>
-      <c r="D60" t="s">
-        <v>219</v>
-      </c>
-    </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>220</v>
+      </c>
+      <c r="B61" t="s">
+        <v>221</v>
+      </c>
+      <c r="C61" t="s">
         <v>222</v>
       </c>
-      <c r="B61" t="s">
+      <c r="D61" t="s">
         <v>223</v>
-      </c>
-      <c r="C61" t="s">
-        <v>224</v>
-      </c>
-      <c r="D61" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B62" t="s">
+        <v>224</v>
+      </c>
+      <c r="C62" t="s">
+        <v>225</v>
+      </c>
+      <c r="D62" t="s">
         <v>226</v>
-      </c>
-      <c r="C62" t="s">
-        <v>227</v>
-      </c>
-      <c r="D62" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B63" t="s">
+        <v>227</v>
+      </c>
+      <c r="C63" t="s">
+        <v>228</v>
+      </c>
+      <c r="D63" t="s">
         <v>229</v>
-      </c>
-      <c r="C63" t="s">
-        <v>230</v>
-      </c>
-      <c r="D63" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B64" t="s">
+        <v>230</v>
+      </c>
+      <c r="C64" t="s">
+        <v>231</v>
+      </c>
+      <c r="D64" t="s">
         <v>232</v>
-      </c>
-      <c r="C64" t="s">
-        <v>233</v>
-      </c>
-      <c r="D64" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B65" t="s">
+        <v>233</v>
+      </c>
+      <c r="C65" t="s">
+        <v>234</v>
+      </c>
+      <c r="D65" t="s">
         <v>235</v>
-      </c>
-      <c r="C65" t="s">
-        <v>236</v>
-      </c>
-      <c r="D65" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B66" t="s">
+        <v>236</v>
+      </c>
+      <c r="C66" t="s">
+        <v>237</v>
+      </c>
+      <c r="D66" t="s">
         <v>238</v>
-      </c>
-      <c r="C66" t="s">
-        <v>239</v>
-      </c>
-      <c r="D66" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B67" t="s">
+        <v>239</v>
+      </c>
+      <c r="C67" t="s">
+        <v>240</v>
+      </c>
+      <c r="D67" t="s">
         <v>241</v>
-      </c>
-      <c r="C67" t="s">
-        <v>242</v>
-      </c>
-      <c r="D67" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B68" t="s">
+        <v>242</v>
+      </c>
+      <c r="C68" t="s">
+        <v>243</v>
+      </c>
+      <c r="D68" t="s">
         <v>244</v>
-      </c>
-      <c r="C68" t="s">
-        <v>245</v>
-      </c>
-      <c r="D68" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B69" t="s">
+        <v>245</v>
+      </c>
+      <c r="C69" t="s">
+        <v>246</v>
+      </c>
+      <c r="D69" t="s">
         <v>247</v>
-      </c>
-      <c r="C69" t="s">
-        <v>248</v>
-      </c>
-      <c r="D69" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B70" t="s">
+        <v>248</v>
+      </c>
+      <c r="C70" t="s">
+        <v>249</v>
+      </c>
+      <c r="D70" t="s">
         <v>250</v>
-      </c>
-      <c r="C70" t="s">
-        <v>251</v>
-      </c>
-      <c r="D70" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B71" t="s">
+        <v>251</v>
+      </c>
+      <c r="C71" t="s">
+        <v>252</v>
+      </c>
+      <c r="D71" t="s">
         <v>253</v>
-      </c>
-      <c r="C71" t="s">
-        <v>254</v>
-      </c>
-      <c r="D71" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B72" t="s">
+        <v>254</v>
+      </c>
+      <c r="C72" t="s">
+        <v>255</v>
+      </c>
+      <c r="D72" t="s">
         <v>256</v>
-      </c>
-      <c r="C72" t="s">
-        <v>257</v>
-      </c>
-      <c r="D72" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B73" t="s">
+        <v>257</v>
+      </c>
+      <c r="C73" t="s">
+        <v>258</v>
+      </c>
+      <c r="D73" t="s">
         <v>259</v>
-      </c>
-      <c r="C73" t="s">
-        <v>260</v>
-      </c>
-      <c r="D73" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B74" t="s">
+        <v>260</v>
+      </c>
+      <c r="C74" t="s">
+        <v>261</v>
+      </c>
+      <c r="D74" t="s">
         <v>262</v>
-      </c>
-      <c r="C74" t="s">
-        <v>263</v>
-      </c>
-      <c r="D74" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B75" t="s">
+        <v>263</v>
+      </c>
+      <c r="C75" t="s">
+        <v>264</v>
+      </c>
+      <c r="D75" t="s">
         <v>265</v>
-      </c>
-      <c r="C75" t="s">
-        <v>266</v>
-      </c>
-      <c r="D75" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B76" t="s">
+        <v>266</v>
+      </c>
+      <c r="C76" t="s">
+        <v>267</v>
+      </c>
+      <c r="D76" t="s">
         <v>268</v>
-      </c>
-      <c r="C76" t="s">
-        <v>269</v>
-      </c>
-      <c r="D76" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B77" t="s">
+        <v>269</v>
+      </c>
+      <c r="C77" t="s">
+        <v>270</v>
+      </c>
+      <c r="D77" t="s">
         <v>271</v>
-      </c>
-      <c r="C77" t="s">
-        <v>272</v>
-      </c>
-      <c r="D77" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B78" t="s">
+        <v>272</v>
+      </c>
+      <c r="C78" t="s">
+        <v>273</v>
+      </c>
+      <c r="D78" t="s">
         <v>274</v>
-      </c>
-      <c r="C78" t="s">
-        <v>275</v>
-      </c>
-      <c r="D78" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2929,13 +2916,13 @@
         <v>5</v>
       </c>
       <c r="B79" t="s">
+        <v>275</v>
+      </c>
+      <c r="C79" t="s">
+        <v>276</v>
+      </c>
+      <c r="D79" t="s">
         <v>277</v>
-      </c>
-      <c r="C79" t="s">
-        <v>278</v>
-      </c>
-      <c r="D79" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2943,69 +2930,69 @@
         <v>5</v>
       </c>
       <c r="B80" t="s">
+        <v>278</v>
+      </c>
+      <c r="C80" t="s">
+        <v>279</v>
+      </c>
+      <c r="D80" t="s">
         <v>280</v>
-      </c>
-      <c r="C80" t="s">
-        <v>281</v>
-      </c>
-      <c r="D80" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>281</v>
+      </c>
+      <c r="B81" t="s">
+        <v>282</v>
+      </c>
+      <c r="C81" t="s">
         <v>283</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>284</v>
-      </c>
-      <c r="C81" t="s">
-        <v>285</v>
-      </c>
-      <c r="D81" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B82" t="s">
+        <v>285</v>
+      </c>
+      <c r="C82" t="s">
+        <v>286</v>
+      </c>
+      <c r="D82" t="s">
         <v>287</v>
-      </c>
-      <c r="C82" t="s">
-        <v>288</v>
-      </c>
-      <c r="D82" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B83" t="s">
+        <v>288</v>
+      </c>
+      <c r="C83" t="s">
+        <v>289</v>
+      </c>
+      <c r="D83" t="s">
         <v>290</v>
-      </c>
-      <c r="C83" t="s">
-        <v>291</v>
-      </c>
-      <c r="D83" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>291</v>
+      </c>
+      <c r="B84" t="s">
+        <v>292</v>
+      </c>
+      <c r="C84" t="s">
         <v>293</v>
       </c>
-      <c r="B84" t="s">
+      <c r="D84" t="s">
         <v>294</v>
-      </c>
-      <c r="C84" t="s">
-        <v>295</v>
-      </c>
-      <c r="D84" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -3013,13 +3000,13 @@
         <v>206</v>
       </c>
       <c r="B85" t="s">
+        <v>295</v>
+      </c>
+      <c r="C85" t="s">
+        <v>296</v>
+      </c>
+      <c r="D85" t="s">
         <v>297</v>
-      </c>
-      <c r="C85" t="s">
-        <v>298</v>
-      </c>
-      <c r="D85" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -3027,10 +3014,10 @@
         <v>206</v>
       </c>
       <c r="C86" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D86" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -3038,13 +3025,13 @@
         <v>40</v>
       </c>
       <c r="B87" t="s">
+        <v>300</v>
+      </c>
+      <c r="C87" t="s">
+        <v>301</v>
+      </c>
+      <c r="D87" t="s">
         <v>302</v>
-      </c>
-      <c r="C87" t="s">
-        <v>303</v>
-      </c>
-      <c r="D87" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -3052,13 +3039,13 @@
         <v>40</v>
       </c>
       <c r="B88" t="s">
+        <v>303</v>
+      </c>
+      <c r="C88" t="s">
+        <v>304</v>
+      </c>
+      <c r="D88" t="s">
         <v>305</v>
-      </c>
-      <c r="C88" t="s">
-        <v>306</v>
-      </c>
-      <c r="D88" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -3066,13 +3053,13 @@
         <v>40</v>
       </c>
       <c r="B89" t="s">
+        <v>306</v>
+      </c>
+      <c r="C89" t="s">
+        <v>307</v>
+      </c>
+      <c r="D89" t="s">
         <v>308</v>
-      </c>
-      <c r="C89" t="s">
-        <v>309</v>
-      </c>
-      <c r="D89" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -3080,13 +3067,13 @@
         <v>40</v>
       </c>
       <c r="B90" t="s">
+        <v>309</v>
+      </c>
+      <c r="C90" t="s">
+        <v>310</v>
+      </c>
+      <c r="D90" t="s">
         <v>311</v>
-      </c>
-      <c r="C90" t="s">
-        <v>312</v>
-      </c>
-      <c r="D90" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -3094,419 +3081,419 @@
         <v>40</v>
       </c>
       <c r="B91" t="s">
+        <v>312</v>
+      </c>
+      <c r="C91" t="s">
+        <v>313</v>
+      </c>
+      <c r="D91" t="s">
         <v>314</v>
-      </c>
-      <c r="C91" t="s">
-        <v>315</v>
-      </c>
-      <c r="D91" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>315</v>
+      </c>
+      <c r="B92" t="s">
+        <v>316</v>
+      </c>
+      <c r="C92" t="s">
         <v>317</v>
       </c>
-      <c r="B92" t="s">
+      <c r="D92" t="s">
         <v>318</v>
-      </c>
-      <c r="C92" t="s">
-        <v>319</v>
-      </c>
-      <c r="D92" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>319</v>
+      </c>
+      <c r="B93" t="s">
+        <v>320</v>
+      </c>
+      <c r="C93" t="s">
         <v>321</v>
       </c>
-      <c r="B93" t="s">
+      <c r="D93" t="s">
         <v>322</v>
-      </c>
-      <c r="C93" t="s">
-        <v>323</v>
-      </c>
-      <c r="D93" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>323</v>
+      </c>
+      <c r="B94" t="s">
+        <v>324</v>
+      </c>
+      <c r="C94" t="s">
         <v>325</v>
       </c>
-      <c r="B94" t="s">
+      <c r="D94" t="s">
         <v>326</v>
-      </c>
-      <c r="C94" t="s">
-        <v>327</v>
-      </c>
-      <c r="D94" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>327</v>
+      </c>
+      <c r="B95" t="s">
+        <v>328</v>
+      </c>
+      <c r="C95" t="s">
         <v>329</v>
       </c>
-      <c r="B95" t="s">
+      <c r="D95" t="s">
         <v>330</v>
-      </c>
-      <c r="C95" t="s">
-        <v>331</v>
-      </c>
-      <c r="D95" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B96" t="s">
+        <v>331</v>
+      </c>
+      <c r="C96" t="s">
+        <v>332</v>
+      </c>
+      <c r="D96" t="s">
         <v>333</v>
-      </c>
-      <c r="C96" t="s">
-        <v>334</v>
-      </c>
-      <c r="D96" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B97" t="s">
+        <v>334</v>
+      </c>
+      <c r="C97" t="s">
+        <v>335</v>
+      </c>
+      <c r="D97" t="s">
         <v>336</v>
-      </c>
-      <c r="C97" t="s">
-        <v>337</v>
-      </c>
-      <c r="D97" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B98" t="s">
+        <v>337</v>
+      </c>
+      <c r="C98" t="s">
+        <v>338</v>
+      </c>
+      <c r="D98" t="s">
         <v>339</v>
-      </c>
-      <c r="C98" t="s">
-        <v>340</v>
-      </c>
-      <c r="D98" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B99" t="s">
+        <v>340</v>
+      </c>
+      <c r="C99" t="s">
+        <v>341</v>
+      </c>
+      <c r="D99" t="s">
         <v>342</v>
-      </c>
-      <c r="C99" t="s">
-        <v>343</v>
-      </c>
-      <c r="D99" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B100" t="s">
+        <v>343</v>
+      </c>
+      <c r="C100" t="s">
+        <v>344</v>
+      </c>
+      <c r="D100" t="s">
         <v>345</v>
-      </c>
-      <c r="C100" t="s">
-        <v>346</v>
-      </c>
-      <c r="D100" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B101" t="s">
+        <v>346</v>
+      </c>
+      <c r="C101" t="s">
+        <v>347</v>
+      </c>
+      <c r="D101" t="s">
         <v>348</v>
-      </c>
-      <c r="C101" t="s">
-        <v>349</v>
-      </c>
-      <c r="D101" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B102" t="s">
+        <v>349</v>
+      </c>
+      <c r="C102" t="s">
+        <v>350</v>
+      </c>
+      <c r="D102" t="s">
         <v>351</v>
-      </c>
-      <c r="C102" t="s">
-        <v>352</v>
-      </c>
-      <c r="D102" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B103" t="s">
+        <v>352</v>
+      </c>
+      <c r="C103" t="s">
+        <v>353</v>
+      </c>
+      <c r="D103" t="s">
         <v>354</v>
-      </c>
-      <c r="C103" t="s">
-        <v>355</v>
-      </c>
-      <c r="D103" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B104" t="s">
+        <v>355</v>
+      </c>
+      <c r="C104" t="s">
+        <v>356</v>
+      </c>
+      <c r="D104" t="s">
         <v>357</v>
-      </c>
-      <c r="C104" t="s">
-        <v>358</v>
-      </c>
-      <c r="D104" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B105" t="s">
+        <v>358</v>
+      </c>
+      <c r="C105" t="s">
+        <v>359</v>
+      </c>
+      <c r="D105" t="s">
         <v>360</v>
-      </c>
-      <c r="C105" t="s">
-        <v>361</v>
-      </c>
-      <c r="D105" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B106" t="s">
+        <v>361</v>
+      </c>
+      <c r="C106" t="s">
+        <v>362</v>
+      </c>
+      <c r="D106" t="s">
         <v>363</v>
-      </c>
-      <c r="C106" t="s">
-        <v>364</v>
-      </c>
-      <c r="D106" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B107" t="s">
+        <v>364</v>
+      </c>
+      <c r="C107" t="s">
+        <v>365</v>
+      </c>
+      <c r="D107" t="s">
         <v>366</v>
-      </c>
-      <c r="C107" t="s">
-        <v>367</v>
-      </c>
-      <c r="D107" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B108" t="s">
+        <v>367</v>
+      </c>
+      <c r="C108" t="s">
+        <v>368</v>
+      </c>
+      <c r="D108" t="s">
         <v>369</v>
-      </c>
-      <c r="C108" t="s">
-        <v>370</v>
-      </c>
-      <c r="D108" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B109" t="s">
+        <v>370</v>
+      </c>
+      <c r="C109" t="s">
+        <v>371</v>
+      </c>
+      <c r="D109" t="s">
         <v>372</v>
-      </c>
-      <c r="C109" t="s">
-        <v>373</v>
-      </c>
-      <c r="D109" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>373</v>
+      </c>
+      <c r="B110" t="s">
+        <v>374</v>
+      </c>
+      <c r="C110" t="s">
         <v>375</v>
       </c>
-      <c r="B110" t="s">
+      <c r="D110" t="s">
         <v>376</v>
-      </c>
-      <c r="C110" t="s">
-        <v>377</v>
-      </c>
-      <c r="D110" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B111" t="s">
+        <v>377</v>
+      </c>
+      <c r="C111" t="s">
+        <v>378</v>
+      </c>
+      <c r="D111" t="s">
         <v>379</v>
-      </c>
-      <c r="C111" t="s">
-        <v>380</v>
-      </c>
-      <c r="D111" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B112" t="s">
+        <v>380</v>
+      </c>
+      <c r="C112" t="s">
+        <v>381</v>
+      </c>
+      <c r="D112" t="s">
         <v>382</v>
-      </c>
-      <c r="C112" t="s">
-        <v>383</v>
-      </c>
-      <c r="D112" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B113" t="s">
+        <v>383</v>
+      </c>
+      <c r="C113" t="s">
+        <v>384</v>
+      </c>
+      <c r="D113" t="s">
         <v>385</v>
-      </c>
-      <c r="C113" t="s">
-        <v>386</v>
-      </c>
-      <c r="D113" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B114" t="s">
+        <v>386</v>
+      </c>
+      <c r="C114" t="s">
+        <v>387</v>
+      </c>
+      <c r="D114" t="s">
         <v>388</v>
-      </c>
-      <c r="C114" t="s">
-        <v>389</v>
-      </c>
-      <c r="D114" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B115" t="s">
+        <v>389</v>
+      </c>
+      <c r="C115" t="s">
+        <v>390</v>
+      </c>
+      <c r="D115" t="s">
         <v>391</v>
-      </c>
-      <c r="C115" t="s">
-        <v>392</v>
-      </c>
-      <c r="D115" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B116" t="s">
+        <v>392</v>
+      </c>
+      <c r="C116" t="s">
+        <v>393</v>
+      </c>
+      <c r="D116" t="s">
         <v>394</v>
-      </c>
-      <c r="C116" t="s">
-        <v>395</v>
-      </c>
-      <c r="D116" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>395</v>
+      </c>
+      <c r="B117" t="s">
+        <v>396</v>
+      </c>
+      <c r="C117" t="s">
         <v>397</v>
       </c>
-      <c r="B117" t="s">
+      <c r="D117" t="s">
         <v>398</v>
-      </c>
-      <c r="C117" t="s">
-        <v>399</v>
-      </c>
-      <c r="D117" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B118" t="s">
+        <v>399</v>
+      </c>
+      <c r="C118" t="s">
+        <v>400</v>
+      </c>
+      <c r="D118" t="s">
         <v>401</v>
-      </c>
-      <c r="C118" t="s">
-        <v>402</v>
-      </c>
-      <c r="D118" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>402</v>
+      </c>
+      <c r="B119" t="s">
+        <v>403</v>
+      </c>
+      <c r="C119" t="s">
         <v>404</v>
       </c>
-      <c r="B119" t="s">
+      <c r="D119" t="s">
         <v>405</v>
-      </c>
-      <c r="C119" t="s">
-        <v>406</v>
-      </c>
-      <c r="D119" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B120" t="s">
+        <v>406</v>
+      </c>
+      <c r="C120" t="s">
+        <v>407</v>
+      </c>
+      <c r="D120" t="s">
         <v>408</v>
-      </c>
-      <c r="C120" t="s">
-        <v>409</v>
-      </c>
-      <c r="D120" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -3514,13 +3501,13 @@
         <v>88</v>
       </c>
       <c r="B121" t="s">
+        <v>409</v>
+      </c>
+      <c r="C121" t="s">
+        <v>410</v>
+      </c>
+      <c r="D121" t="s">
         <v>411</v>
-      </c>
-      <c r="C121" t="s">
-        <v>412</v>
-      </c>
-      <c r="D121" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -3539,7 +3526,7 @@
         <v>77</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C123" s="2">
         <v>163540</v>
@@ -3550,10 +3537,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C124" s="2">
         <v>51165</v>
@@ -3567,7 +3554,7 @@
         <v>67</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C125" s="2">
         <v>32029</v>
@@ -3577,25 +3564,17 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="C126" s="2">
-        <v>54044</v>
-      </c>
-      <c r="D126" s="2">
-        <v>2305310</v>
-      </c>
+      <c r="A126" s="2"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="2"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C127" s="2">
         <v>37304</v>
@@ -3609,7 +3588,7 @@
         <v>67</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C128" s="2">
         <v>32031</v>
@@ -3623,7 +3602,7 @@
         <v>67</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C129" s="2">
         <v>167273</v>
@@ -3637,7 +3616,7 @@
         <v>167</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C130" s="2">
         <v>1035443</v>
@@ -3651,7 +3630,7 @@
         <v>40</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C131" s="2">
         <v>42008</v>
@@ -3662,10 +3641,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C132" s="2">
         <v>38322</v>
@@ -3685,7 +3664,7 @@
         <v>1706510</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="134" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -3704,13 +3683,13 @@
         <v>5</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C135" s="4">
         <v>161679</v>
       </c>
       <c r="D135" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -3718,7 +3697,7 @@
         <v>5</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C136" s="4">
         <v>1268305</v>
@@ -3729,10 +3708,10 @@
     </row>
     <row r="137" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C137">
         <v>38320</v>
@@ -3743,7 +3722,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C138" s="4">
         <v>108426</v>
@@ -3779,7 +3758,7 @@
         <v>123</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C141" s="4">
         <v>1269433</v>
@@ -3793,7 +3772,7 @@
         <v>123</v>
       </c>
       <c r="B142" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C142" s="4">
         <v>1270508</v>
@@ -3804,13 +3783,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C143" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D143" s="4">
         <v>2314794</v>
@@ -3821,10 +3800,10 @@
         <v>123</v>
       </c>
       <c r="B144" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C144" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D144" s="4">
         <v>602670</v>
@@ -3835,13 +3814,62 @@
         <v>123</v>
       </c>
       <c r="B145" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C145" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D145" s="4">
         <v>636390</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146">
+        <v>161836</v>
+      </c>
+      <c r="D146" s="9">
+        <v>2680930</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147">
+        <v>161839</v>
+      </c>
+      <c r="D147" s="9">
+        <v>2630390</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>435</v>
+      </c>
+      <c r="C148" s="9">
+        <v>229992</v>
+      </c>
+      <c r="D148" s="9">
+        <v>504020</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C149">
+        <v>98679</v>
+      </c>
+      <c r="D149" s="9">
+        <v>565760</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C150">
+        <v>196564</v>
+      </c>
+      <c r="D150" s="9">
+        <v>1736600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
consolidated some schools, update ncesID
</commit_message>
<xml_diff>
--- a/data/_dictionary_13.xlsx
+++ b/data/_dictionary_13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/acfrs_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA3FBB6-00CF-484B-8A7F-57086BFA088A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD28667-B327-8D40-9822-7D92907F987D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6300" windowWidth="24120" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7920" windowWidth="21380" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="463">
   <si>
     <t>state.abb</t>
   </si>
@@ -1356,13 +1356,79 @@
   </si>
   <si>
     <t>bristol-plymouth regional technical school district</t>
+  </si>
+  <si>
+    <t>san bernardino county superintendent of schools</t>
+  </si>
+  <si>
+    <t>chippewa falls area unified school district</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>bokoshe independent school district no. 26</t>
+  </si>
+  <si>
+    <t>south river borough board of education</t>
+  </si>
+  <si>
+    <t>town of westfield school district (union county)</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>chickasaw county school district</t>
+  </si>
+  <si>
+    <t>menifee county school district</t>
+  </si>
+  <si>
+    <t>school district of the city of muskegon heights</t>
+  </si>
+  <si>
+    <t>scotts bluff county school district no. 16</t>
+  </si>
+  <si>
+    <t>swedesboro-woolwich consolidated school district</t>
+  </si>
+  <si>
+    <t>school district of grantsburg</t>
+  </si>
+  <si>
+    <t>school district of sheboygan falls</t>
+  </si>
+  <si>
+    <t>grafton public school district no. 18</t>
+  </si>
+  <si>
+    <t>skiatook independent school district no. 7</t>
+  </si>
+  <si>
+    <t>school district of mayville</t>
+  </si>
+  <si>
+    <t>metuchen public schools</t>
+  </si>
+  <si>
+    <t>somers public school</t>
+  </si>
+  <si>
+    <t>mountainside school district</t>
+  </si>
+  <si>
+    <t>jones independent school district no. 9</t>
+  </si>
+  <si>
+    <t>school district of north fond du lac</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1421,6 +1487,18 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1454,7 +1532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1469,6 +1547,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1773,11 +1856,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E178"/>
+  <dimension ref="A1:E203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D171" sqref="D171"/>
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G191" sqref="G191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3547,18 +3630,10 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A125" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="C125" s="2">
-        <v>32029</v>
-      </c>
-      <c r="D125" s="2">
-        <v>800272</v>
-      </c>
+      <c r="A125" s="2"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
@@ -4182,6 +4257,338 @@
         <v>3409990</v>
       </c>
     </row>
+    <row r="179" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B179" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="C179" s="10">
+        <v>1267593</v>
+      </c>
+      <c r="D179" s="10">
+        <v>691029</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B180" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="C180" s="10">
+        <v>32029</v>
+      </c>
+      <c r="D180" s="10">
+        <v>801950</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="B181" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="C181" s="13">
+        <v>39946</v>
+      </c>
+      <c r="D181" s="13">
+        <v>5502550</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C182">
+        <v>1238297</v>
+      </c>
+      <c r="D182">
+        <v>2012360</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C183" s="9">
+        <v>197115</v>
+      </c>
+      <c r="D183" s="9">
+        <v>3629910</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C184" s="9">
+        <v>190589</v>
+      </c>
+      <c r="D184" s="9">
+        <v>3613110</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B185" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="C185" s="9">
+        <v>44406</v>
+      </c>
+      <c r="D185" s="9">
+        <v>4004950</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B186" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="C186" s="13">
+        <v>35819</v>
+      </c>
+      <c r="D186" s="13">
+        <v>3415390</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="B187" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="C187" s="16">
+        <v>48337</v>
+      </c>
+      <c r="D187" s="9">
+        <v>5510740</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B188" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="C188" s="15">
+        <v>82103</v>
+      </c>
+      <c r="D188" s="9">
+        <v>3417760</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" s="15" t="s">
+        <v>447</v>
+      </c>
+      <c r="B189" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="C189" s="15">
+        <v>34992</v>
+      </c>
+      <c r="D189" s="13">
+        <v>2800200</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B190" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="C190" s="15">
+        <v>33713</v>
+      </c>
+      <c r="D190" s="9">
+        <v>2104080</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B191" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="C191" s="15">
+        <v>161783</v>
+      </c>
+      <c r="D191" s="9">
+        <v>2624870</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B192" s="15" t="s">
+        <v>451</v>
+      </c>
+      <c r="C192" s="15">
+        <v>93980</v>
+      </c>
+      <c r="D192" s="13">
+        <v>3176470</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B193" s="15" t="s">
+        <v>452</v>
+      </c>
+      <c r="C193" s="15">
+        <v>282523</v>
+      </c>
+      <c r="D193" s="13">
+        <v>3415990</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="B194" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="C194" s="15">
+        <v>48416</v>
+      </c>
+      <c r="D194" s="9">
+        <v>5505670</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="B195" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="C195" s="15">
+        <v>45309</v>
+      </c>
+      <c r="D195" s="15">
+        <v>5513680</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="B196" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="C196" s="15">
+        <v>1239333</v>
+      </c>
+      <c r="D196" s="15">
+        <v>3800406</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="B197" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="C197" s="15">
+        <v>1239251</v>
+      </c>
+      <c r="D197" s="15">
+        <v>4027750</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="B198" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="C198" s="15">
+        <v>45097</v>
+      </c>
+      <c r="D198" s="15">
+        <v>5508880</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B199" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="C199" s="15">
+        <v>35814</v>
+      </c>
+      <c r="D199" s="15">
+        <v>3409990</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B200" s="15" t="s">
+        <v>459</v>
+      </c>
+      <c r="C200" s="15">
+        <v>398575</v>
+      </c>
+      <c r="D200" s="15">
+        <v>3000002</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B201" s="15" t="s">
+        <v>460</v>
+      </c>
+      <c r="C201" s="15">
+        <v>1265965</v>
+      </c>
+      <c r="D201" s="15">
+        <v>3411040</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="B202" s="15" t="s">
+        <v>461</v>
+      </c>
+      <c r="C202" s="15">
+        <v>37452</v>
+      </c>
+      <c r="D202" s="15">
+        <v>4015840</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C203" s="15">
+        <v>32029</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix hettinger ND, update query counties, muni
</commit_message>
<xml_diff>
--- a/data/_dictionary_13.xlsx
+++ b/data/_dictionary_13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/acfrs_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD28667-B327-8D40-9822-7D92907F987D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76EC911-150F-8C4E-AB5D-8E1314310529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7920" windowWidth="21380" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7900" windowWidth="21380" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="462">
   <si>
     <t>state.abb</t>
   </si>
@@ -1341,9 +1341,6 @@
   </si>
   <si>
     <t>sayreville borough school district</t>
-  </si>
-  <si>
-    <t>bamberg county school district</t>
   </si>
   <si>
     <t>north brunswick board of education</t>
@@ -1859,8 +1856,8 @@
   <dimension ref="A1:E203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G191" sqref="G191"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B205" sqref="B205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3793,15 +3790,9 @@
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="C138" s="4">
-        <v>108426</v>
-      </c>
-      <c r="D138" s="4">
-        <v>3800406</v>
-      </c>
+      <c r="A138" s="2"/>
+      <c r="C138" s="4"/>
+      <c r="D138" s="4"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
@@ -4051,15 +4042,8 @@
       <c r="D162" s="4"/>
     </row>
     <row r="163" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C163" s="4">
-        <v>1270501</v>
-      </c>
-      <c r="D163" s="4">
-        <v>3409990</v>
-      </c>
+      <c r="C163" s="4"/>
+      <c r="D163" s="4"/>
     </row>
     <row r="164" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
@@ -4174,18 +4158,10 @@
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A173" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="B173" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="C173" s="10">
-        <v>1268144</v>
-      </c>
-      <c r="D173" s="4">
-        <v>4503916</v>
-      </c>
+      <c r="A173" s="10"/>
+      <c r="B173" s="10"/>
+      <c r="C173" s="10"/>
+      <c r="D173" s="4"/>
       <c r="E173" s="5"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -4193,7 +4169,7 @@
         <v>40</v>
       </c>
       <c r="B174" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C174" s="10">
         <v>225175</v>
@@ -4208,7 +4184,7 @@
         <v>388</v>
       </c>
       <c r="B175" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C175" s="10">
         <v>37827</v>
@@ -4223,7 +4199,7 @@
         <v>21</v>
       </c>
       <c r="B176" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C176" s="10">
         <v>168178</v>
@@ -4237,7 +4213,7 @@
         <v>55</v>
       </c>
       <c r="B177" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C177" s="10">
         <v>34198</v>
@@ -4247,22 +4223,16 @@
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A178" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C178" s="4">
-        <v>1240267</v>
-      </c>
-      <c r="D178" s="4">
-        <v>3409990</v>
-      </c>
+      <c r="A178" s="10"/>
+      <c r="C178" s="4"/>
+      <c r="D178" s="4"/>
     </row>
     <row r="179" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A179" s="10" t="s">
         <v>123</v>
       </c>
       <c r="B179" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C179" s="10">
         <v>1267593</v>
@@ -4287,10 +4257,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C181" s="13">
         <v>39946</v>
@@ -4337,7 +4307,7 @@
         <v>320</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C185" s="9">
         <v>44406</v>
@@ -4351,7 +4321,7 @@
         <v>40</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C186" s="13">
         <v>35819</v>
@@ -4362,10 +4332,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B187" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C187" s="16">
         <v>48337</v>
@@ -4379,7 +4349,7 @@
         <v>40</v>
       </c>
       <c r="B188" s="15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C188" s="15">
         <v>82103</v>
@@ -4390,10 +4360,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="B189" s="15" t="s">
         <v>447</v>
-      </c>
-      <c r="B189" s="15" t="s">
-        <v>448</v>
       </c>
       <c r="C189" s="15">
         <v>34992</v>
@@ -4407,7 +4377,7 @@
         <v>31</v>
       </c>
       <c r="B190" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C190" s="15">
         <v>33713</v>
@@ -4421,7 +4391,7 @@
         <v>5</v>
       </c>
       <c r="B191" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C191" s="15">
         <v>161783</v>
@@ -4435,7 +4405,7 @@
         <v>202</v>
       </c>
       <c r="B192" s="15" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C192" s="15">
         <v>93980</v>
@@ -4449,7 +4419,7 @@
         <v>40</v>
       </c>
       <c r="B193" s="15" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C193" s="15">
         <v>282523</v>
@@ -4460,10 +4430,10 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B194" s="15" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C194" s="15">
         <v>48416</v>
@@ -4474,10 +4444,10 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B195" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C195" s="15">
         <v>45309</v>
@@ -4491,7 +4461,7 @@
         <v>419</v>
       </c>
       <c r="B196" s="15" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C196" s="15">
         <v>1239333</v>
@@ -4505,7 +4475,7 @@
         <v>320</v>
       </c>
       <c r="B197" s="15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C197" s="15">
         <v>1239251</v>
@@ -4516,10 +4486,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B198" s="15" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C198" s="15">
         <v>45097</v>
@@ -4533,7 +4503,7 @@
         <v>40</v>
       </c>
       <c r="B199" s="15" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C199" s="15">
         <v>35814</v>
@@ -4547,7 +4517,7 @@
         <v>110</v>
       </c>
       <c r="B200" s="15" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C200" s="15">
         <v>398575</v>
@@ -4561,7 +4531,7 @@
         <v>40</v>
       </c>
       <c r="B201" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C201" s="15">
         <v>1265965</v>
@@ -4575,7 +4545,7 @@
         <v>320</v>
       </c>
       <c r="B202" s="15" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C202" s="15">
         <v>37452</v>
@@ -4585,9 +4555,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C203" s="15">
-        <v>32029</v>
-      </c>
+      <c r="C203" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix ncesID of some sd in IN
</commit_message>
<xml_diff>
--- a/data/_dictionary_13.xlsx
+++ b/data/_dictionary_13.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/acfrs_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76EC911-150F-8C4E-AB5D-8E1314310529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65BD9B1-8E3D-E042-8E0F-064F929844A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7900" windowWidth="21380" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3260" windowWidth="21380" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="463">
   <si>
     <t>state.abb</t>
   </si>
@@ -617,9 +616,6 @@
     <t>107774</t>
   </si>
   <si>
-    <t>1802040</t>
-  </si>
-  <si>
     <t>northwestern consolidated school district of shelby county</t>
   </si>
   <si>
@@ -1419,13 +1415,19 @@
   </si>
   <si>
     <t>school district of north fond du lac</t>
+  </si>
+  <si>
+    <t>muncie community schools</t>
+  </si>
+  <si>
+    <t>northwestern school corp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1496,6 +1498,17 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1529,7 +1542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1549,6 +1562,8 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1853,17 +1868,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E203"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B205" sqref="B205"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D206" sqref="D206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="58.1640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -2662,8 +2677,8 @@
       <c r="C53" t="s">
         <v>193</v>
       </c>
-      <c r="D53" t="s">
-        <v>194</v>
+      <c r="D53" s="17">
+        <v>1808310</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2671,321 +2686,321 @@
         <v>191</v>
       </c>
       <c r="B54" t="s">
+        <v>194</v>
+      </c>
+      <c r="C54" t="s">
         <v>195</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>196</v>
-      </c>
-      <c r="D54" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>197</v>
+      </c>
+      <c r="B55" t="s">
         <v>198</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>199</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>200</v>
-      </c>
-      <c r="D55" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>202</v>
+      </c>
+      <c r="B57" t="s">
         <v>203</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>204</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>205</v>
-      </c>
-      <c r="D57" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B58" t="s">
+        <v>206</v>
+      </c>
+      <c r="C58" t="s">
         <v>207</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>208</v>
-      </c>
-      <c r="D58" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B59" t="s">
+        <v>209</v>
+      </c>
+      <c r="C59" t="s">
         <v>210</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>211</v>
-      </c>
-      <c r="D59" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>212</v>
+      </c>
+      <c r="B61" t="s">
         <v>213</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>214</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>215</v>
-      </c>
-      <c r="D61" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B62" t="s">
+        <v>216</v>
+      </c>
+      <c r="C62" t="s">
         <v>217</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>218</v>
-      </c>
-      <c r="D62" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B63" t="s">
+        <v>219</v>
+      </c>
+      <c r="C63" t="s">
         <v>220</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>221</v>
-      </c>
-      <c r="D63" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B64" t="s">
+        <v>222</v>
+      </c>
+      <c r="C64" t="s">
         <v>223</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>224</v>
-      </c>
-      <c r="D64" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B65" t="s">
+        <v>225</v>
+      </c>
+      <c r="C65" t="s">
         <v>226</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>227</v>
-      </c>
-      <c r="D65" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B66" t="s">
+        <v>228</v>
+      </c>
+      <c r="C66" t="s">
         <v>229</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>230</v>
-      </c>
-      <c r="D66" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B67" t="s">
+        <v>231</v>
+      </c>
+      <c r="C67" t="s">
         <v>232</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>233</v>
-      </c>
-      <c r="D67" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B68" t="s">
+        <v>234</v>
+      </c>
+      <c r="C68" t="s">
         <v>235</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>236</v>
-      </c>
-      <c r="D68" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B69" t="s">
+        <v>237</v>
+      </c>
+      <c r="C69" t="s">
         <v>238</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>239</v>
-      </c>
-      <c r="D69" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B70" t="s">
+        <v>240</v>
+      </c>
+      <c r="C70" t="s">
         <v>241</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>242</v>
-      </c>
-      <c r="D70" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B71" t="s">
+        <v>243</v>
+      </c>
+      <c r="C71" t="s">
         <v>244</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>245</v>
-      </c>
-      <c r="D71" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B72" t="s">
+        <v>246</v>
+      </c>
+      <c r="C72" t="s">
         <v>247</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>248</v>
-      </c>
-      <c r="D72" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B73" t="s">
+        <v>249</v>
+      </c>
+      <c r="C73" t="s">
         <v>250</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>251</v>
-      </c>
-      <c r="D73" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B74" t="s">
+        <v>252</v>
+      </c>
+      <c r="C74" t="s">
         <v>253</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>254</v>
-      </c>
-      <c r="D74" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B75" t="s">
+        <v>255</v>
+      </c>
+      <c r="C75" t="s">
         <v>256</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>257</v>
-      </c>
-      <c r="D75" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B76" t="s">
+        <v>258</v>
+      </c>
+      <c r="C76" t="s">
         <v>259</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>260</v>
-      </c>
-      <c r="D76" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B77" t="s">
+        <v>261</v>
+      </c>
+      <c r="C77" t="s">
         <v>262</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>263</v>
-      </c>
-      <c r="D77" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B78" t="s">
+        <v>264</v>
+      </c>
+      <c r="C78" t="s">
         <v>265</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>266</v>
-      </c>
-      <c r="D78" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2993,13 +3008,13 @@
         <v>5</v>
       </c>
       <c r="B79" t="s">
+        <v>267</v>
+      </c>
+      <c r="C79" t="s">
         <v>268</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>269</v>
-      </c>
-      <c r="D79" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -3007,94 +3022,94 @@
         <v>5</v>
       </c>
       <c r="B80" t="s">
+        <v>270</v>
+      </c>
+      <c r="C80" t="s">
         <v>271</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>272</v>
-      </c>
-      <c r="D80" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>273</v>
+      </c>
+      <c r="B81" t="s">
         <v>274</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>275</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>276</v>
-      </c>
-      <c r="D81" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B82" t="s">
+        <v>277</v>
+      </c>
+      <c r="C82" t="s">
         <v>278</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>279</v>
-      </c>
-      <c r="D82" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B83" t="s">
+        <v>280</v>
+      </c>
+      <c r="C83" t="s">
         <v>281</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>282</v>
-      </c>
-      <c r="D83" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>283</v>
+      </c>
+      <c r="B84" t="s">
         <v>284</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>285</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>286</v>
-      </c>
-      <c r="D84" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B85" t="s">
+        <v>287</v>
+      </c>
+      <c r="C85" t="s">
         <v>288</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>289</v>
-      </c>
-      <c r="D85" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C86" t="s">
+        <v>290</v>
+      </c>
+      <c r="D86" t="s">
         <v>291</v>
-      </c>
-      <c r="D86" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -3102,13 +3117,13 @@
         <v>40</v>
       </c>
       <c r="B87" t="s">
+        <v>292</v>
+      </c>
+      <c r="C87" t="s">
         <v>293</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>294</v>
-      </c>
-      <c r="D87" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -3116,13 +3131,13 @@
         <v>40</v>
       </c>
       <c r="B88" t="s">
+        <v>295</v>
+      </c>
+      <c r="C88" t="s">
         <v>296</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>297</v>
-      </c>
-      <c r="D88" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -3130,13 +3145,13 @@
         <v>40</v>
       </c>
       <c r="B89" t="s">
+        <v>298</v>
+      </c>
+      <c r="C89" t="s">
         <v>299</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>300</v>
-      </c>
-      <c r="D89" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -3144,13 +3159,13 @@
         <v>40</v>
       </c>
       <c r="B90" t="s">
+        <v>301</v>
+      </c>
+      <c r="C90" t="s">
         <v>302</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>303</v>
-      </c>
-      <c r="D90" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -3158,419 +3173,419 @@
         <v>40</v>
       </c>
       <c r="B91" t="s">
+        <v>304</v>
+      </c>
+      <c r="C91" t="s">
         <v>305</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>306</v>
-      </c>
-      <c r="D91" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>307</v>
+      </c>
+      <c r="B92" t="s">
         <v>308</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>309</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>310</v>
-      </c>
-      <c r="D92" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>311</v>
+      </c>
+      <c r="B93" t="s">
         <v>312</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>313</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>314</v>
-      </c>
-      <c r="D93" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>315</v>
+      </c>
+      <c r="B94" t="s">
         <v>316</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>317</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>318</v>
-      </c>
-      <c r="D94" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>319</v>
+      </c>
+      <c r="B95" t="s">
         <v>320</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>321</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>322</v>
-      </c>
-      <c r="D95" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B96" t="s">
+        <v>323</v>
+      </c>
+      <c r="C96" t="s">
         <v>324</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>325</v>
-      </c>
-      <c r="D96" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B97" t="s">
+        <v>326</v>
+      </c>
+      <c r="C97" t="s">
         <v>327</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>328</v>
-      </c>
-      <c r="D97" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B98" t="s">
+        <v>329</v>
+      </c>
+      <c r="C98" t="s">
         <v>330</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>331</v>
-      </c>
-      <c r="D98" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B99" t="s">
+        <v>332</v>
+      </c>
+      <c r="C99" t="s">
         <v>333</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>334</v>
-      </c>
-      <c r="D99" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B100" t="s">
+        <v>335</v>
+      </c>
+      <c r="C100" t="s">
         <v>336</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
         <v>337</v>
-      </c>
-      <c r="D100" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B101" t="s">
+        <v>338</v>
+      </c>
+      <c r="C101" t="s">
         <v>339</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>340</v>
-      </c>
-      <c r="D101" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B102" t="s">
+        <v>341</v>
+      </c>
+      <c r="C102" t="s">
         <v>342</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>343</v>
-      </c>
-      <c r="D102" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B103" t="s">
+        <v>344</v>
+      </c>
+      <c r="C103" t="s">
         <v>345</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>346</v>
-      </c>
-      <c r="D103" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B104" t="s">
+        <v>347</v>
+      </c>
+      <c r="C104" t="s">
         <v>348</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
         <v>349</v>
-      </c>
-      <c r="D104" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B105" t="s">
+        <v>350</v>
+      </c>
+      <c r="C105" t="s">
         <v>351</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
         <v>352</v>
-      </c>
-      <c r="D105" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B106" t="s">
+        <v>353</v>
+      </c>
+      <c r="C106" t="s">
         <v>354</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
         <v>355</v>
-      </c>
-      <c r="D106" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B107" t="s">
+        <v>356</v>
+      </c>
+      <c r="C107" t="s">
         <v>357</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" t="s">
         <v>358</v>
-      </c>
-      <c r="D107" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B108" t="s">
+        <v>359</v>
+      </c>
+      <c r="C108" t="s">
         <v>360</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
         <v>361</v>
-      </c>
-      <c r="D108" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B109" t="s">
+        <v>362</v>
+      </c>
+      <c r="C109" t="s">
         <v>363</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>364</v>
-      </c>
-      <c r="D109" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>365</v>
+      </c>
+      <c r="B110" t="s">
         <v>366</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>367</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
         <v>368</v>
-      </c>
-      <c r="D110" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B111" t="s">
+        <v>369</v>
+      </c>
+      <c r="C111" t="s">
         <v>370</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>371</v>
-      </c>
-      <c r="D111" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B112" t="s">
+        <v>372</v>
+      </c>
+      <c r="C112" t="s">
         <v>373</v>
       </c>
-      <c r="C112" t="s">
+      <c r="D112" t="s">
         <v>374</v>
-      </c>
-      <c r="D112" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B113" t="s">
+        <v>375</v>
+      </c>
+      <c r="C113" t="s">
         <v>376</v>
       </c>
-      <c r="C113" t="s">
+      <c r="D113" t="s">
         <v>377</v>
-      </c>
-      <c r="D113" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B114" t="s">
+        <v>378</v>
+      </c>
+      <c r="C114" t="s">
         <v>379</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D114" t="s">
         <v>380</v>
-      </c>
-      <c r="D114" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B115" t="s">
+        <v>381</v>
+      </c>
+      <c r="C115" t="s">
         <v>382</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
         <v>383</v>
-      </c>
-      <c r="D115" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B116" t="s">
+        <v>384</v>
+      </c>
+      <c r="C116" t="s">
         <v>385</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
         <v>386</v>
-      </c>
-      <c r="D116" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>387</v>
+      </c>
+      <c r="B117" t="s">
         <v>388</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>389</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
         <v>390</v>
-      </c>
-      <c r="D117" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B118" t="s">
+        <v>391</v>
+      </c>
+      <c r="C118" t="s">
         <v>392</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
         <v>393</v>
-      </c>
-      <c r="D118" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>394</v>
+      </c>
+      <c r="B119" t="s">
         <v>395</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>396</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
         <v>397</v>
-      </c>
-      <c r="D119" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B120" t="s">
+        <v>398</v>
+      </c>
+      <c r="C120" t="s">
         <v>399</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" t="s">
         <v>400</v>
-      </c>
-      <c r="D120" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -3578,18 +3593,18 @@
         <v>88</v>
       </c>
       <c r="B121" t="s">
+        <v>401</v>
+      </c>
+      <c r="C121" t="s">
         <v>402</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" t="s">
         <v>403</v>
-      </c>
-      <c r="D121" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C122">
         <v>224518</v>
@@ -3603,7 +3618,7 @@
         <v>77</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C123" s="2">
         <v>163540</v>
@@ -3614,10 +3629,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C124" s="2">
         <v>51165</v>
@@ -3640,10 +3655,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C127" s="2">
         <v>37304</v>
@@ -3657,7 +3672,7 @@
         <v>67</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C128" s="2">
         <v>32031</v>
@@ -3671,7 +3686,7 @@
         <v>67</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C129" s="2">
         <v>167273</v>
@@ -3685,7 +3700,7 @@
         <v>163</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C130" s="2">
         <v>1035443</v>
@@ -3699,7 +3714,7 @@
         <v>40</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C131" s="2">
         <v>42008</v>
@@ -3710,10 +3725,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C132" s="2">
         <v>38322</v>
@@ -3733,7 +3748,7 @@
         <v>1706510</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="134" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -3752,13 +3767,13 @@
         <v>5</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C135" s="4">
         <v>161679</v>
       </c>
       <c r="D135" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -3766,7 +3781,7 @@
         <v>5</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C136" s="4">
         <v>1268305</v>
@@ -3777,10 +3792,10 @@
     </row>
     <row r="137" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C137">
         <v>38320</v>
@@ -3821,7 +3836,7 @@
         <v>123</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C141" s="4">
         <v>1269433</v>
@@ -3837,13 +3852,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B143" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="C143" t="s">
         <v>421</v>
-      </c>
-      <c r="C143" t="s">
-        <v>422</v>
       </c>
       <c r="D143" s="4">
         <v>2314794</v>
@@ -3854,10 +3869,10 @@
         <v>123</v>
       </c>
       <c r="B144" t="s">
+        <v>422</v>
+      </c>
+      <c r="C144" t="s">
         <v>423</v>
-      </c>
-      <c r="C144" t="s">
-        <v>424</v>
       </c>
       <c r="D144" s="4">
         <v>602670</v>
@@ -3868,10 +3883,10 @@
         <v>123</v>
       </c>
       <c r="B145" t="s">
+        <v>424</v>
+      </c>
+      <c r="C145" t="s">
         <v>425</v>
-      </c>
-      <c r="C145" t="s">
-        <v>426</v>
       </c>
       <c r="D145" s="4">
         <v>636390</v>
@@ -3901,7 +3916,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C148" s="9">
         <v>229992</v>
@@ -3923,10 +3938,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
+        <v>427</v>
+      </c>
+      <c r="B151" s="4" t="s">
         <v>428</v>
-      </c>
-      <c r="B151" s="4" t="s">
-        <v>429</v>
       </c>
       <c r="C151" s="4">
         <v>1035255</v>
@@ -3959,7 +3974,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C154">
         <v>190314</v>
@@ -3981,7 +3996,7 @@
     </row>
     <row r="156" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C156" s="5">
         <v>146931</v>
@@ -3992,7 +4007,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C157">
         <v>56143</v>
@@ -4003,7 +4018,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C158">
         <v>1027279</v>
@@ -4058,7 +4073,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C165" s="4">
         <v>37850</v>
@@ -4074,10 +4089,10 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B167" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C167" s="10">
         <v>42811</v>
@@ -4092,7 +4107,7 @@
         <v>21</v>
       </c>
       <c r="B168" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C168" s="10">
         <v>36466</v>
@@ -4106,7 +4121,7 @@
         <v>88</v>
       </c>
       <c r="B169" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C169" s="10">
         <v>39597</v>
@@ -4120,7 +4135,7 @@
         <v>40</v>
       </c>
       <c r="B170" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C170" s="4">
         <v>35783</v>
@@ -4131,10 +4146,10 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B171" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C171" s="10">
         <v>42478</v>
@@ -4148,7 +4163,7 @@
         <v>40</v>
       </c>
       <c r="B172" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C172" s="10">
         <v>35817</v>
@@ -4169,7 +4184,7 @@
         <v>40</v>
       </c>
       <c r="B174" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C174" s="10">
         <v>225175</v>
@@ -4181,10 +4196,10 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B175" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C175" s="10">
         <v>37827</v>
@@ -4199,7 +4214,7 @@
         <v>21</v>
       </c>
       <c r="B176" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C176" s="10">
         <v>168178</v>
@@ -4213,7 +4228,7 @@
         <v>55</v>
       </c>
       <c r="B177" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C177" s="10">
         <v>34198</v>
@@ -4232,7 +4247,7 @@
         <v>123</v>
       </c>
       <c r="B179" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C179" s="10">
         <v>1267593</v>
@@ -4246,7 +4261,7 @@
         <v>67</v>
       </c>
       <c r="B180" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C180" s="10">
         <v>32029</v>
@@ -4257,10 +4272,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C181" s="13">
         <v>39946</v>
@@ -4271,7 +4286,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C182">
         <v>1238297</v>
@@ -4304,10 +4319,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C185" s="9">
         <v>44406</v>
@@ -4321,7 +4336,7 @@
         <v>40</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C186" s="13">
         <v>35819</v>
@@ -4332,10 +4347,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B187" s="15" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C187" s="16">
         <v>48337</v>
@@ -4349,7 +4364,7 @@
         <v>40</v>
       </c>
       <c r="B188" s="15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C188" s="15">
         <v>82103</v>
@@ -4360,10 +4375,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="B189" s="15" t="s">
         <v>446</v>
-      </c>
-      <c r="B189" s="15" t="s">
-        <v>447</v>
       </c>
       <c r="C189" s="15">
         <v>34992</v>
@@ -4377,7 +4392,7 @@
         <v>31</v>
       </c>
       <c r="B190" s="15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C190" s="15">
         <v>33713</v>
@@ -4391,7 +4406,7 @@
         <v>5</v>
       </c>
       <c r="B191" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C191" s="15">
         <v>161783</v>
@@ -4402,10 +4417,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B192" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C192" s="15">
         <v>93980</v>
@@ -4419,7 +4434,7 @@
         <v>40</v>
       </c>
       <c r="B193" s="15" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C193" s="15">
         <v>282523</v>
@@ -4430,10 +4445,10 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B194" s="15" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C194" s="15">
         <v>48416</v>
@@ -4444,10 +4459,10 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B195" s="15" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C195" s="15">
         <v>45309</v>
@@ -4458,10 +4473,10 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B196" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C196" s="15">
         <v>1239333</v>
@@ -4472,10 +4487,10 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B197" s="15" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C197" s="15">
         <v>1239251</v>
@@ -4486,10 +4501,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B198" s="15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C198" s="15">
         <v>45097</v>
@@ -4503,7 +4518,7 @@
         <v>40</v>
       </c>
       <c r="B199" s="15" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C199" s="15">
         <v>35814</v>
@@ -4517,7 +4532,7 @@
         <v>110</v>
       </c>
       <c r="B200" s="15" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C200" s="15">
         <v>398575</v>
@@ -4531,7 +4546,7 @@
         <v>40</v>
       </c>
       <c r="B201" s="15" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C201" s="15">
         <v>1265965</v>
@@ -4542,10 +4557,10 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B202" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C202" s="15">
         <v>37452</v>
@@ -4555,7 +4570,32 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C203" s="15"/>
+      <c r="A203" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B203" s="17" t="s">
+        <v>461</v>
+      </c>
+      <c r="C203" s="17">
+        <v>43699</v>
+      </c>
+      <c r="D203" s="17">
+        <v>1807320</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B204" s="17" t="s">
+        <v>462</v>
+      </c>
+      <c r="C204" s="17">
+        <v>93917</v>
+      </c>
+      <c r="D204" s="17">
+        <v>1802040</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>